<commit_message>
Added logging and refactored code.
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48" count="14472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66" count="17102">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -155,6 +155,60 @@
   </si>
   <si>
     <t>063-536-00-23</t>
+  </si>
+  <si>
+    <t>Країна слідування</t>
+  </si>
+  <si>
+    <t>dfqfg</t>
+  </si>
+  <si>
+    <t>Дата та місце(пункт пропуску) перетину державного кордону України</t>
+  </si>
+  <si>
+    <t>fveda</t>
+  </si>
+  <si>
+    <t>Запланована дата та місце(пункт пропуску) перетину державного кордону України в зворотному напрямку</t>
+  </si>
+  <si>
+    <t>Fevd fg</t>
+  </si>
+  <si>
+    <t>ПІБ керівника самостійного структурного підрозділу,телефон,особистий підпис і дата</t>
+  </si>
+  <si>
+    <t>ніе</t>
+  </si>
+  <si>
+    <t>ПІБ,дата народження,номер телефону</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>Підрозділ війсковослужбовця</t>
+  </si>
+  <si>
+    <t>муек</t>
+  </si>
+  <si>
+    <t>Підстава для виїзду:дата та №(рішення)</t>
+  </si>
+  <si>
+    <t>кме</t>
+  </si>
+  <si>
+    <t>кпим</t>
+  </si>
+  <si>
+    <t>ва</t>
+  </si>
+  <si>
+    <t>кмафвіма</t>
+  </si>
+  <si>
+    <t>вуман</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I808"/>
+  <dimension ref="A1:I963"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -22378,27 +22432,3841 @@
     </row>
     <row r="808">
       <c r="A808" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C808" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D808" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E808" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F808" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G808" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H808" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B809" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C809" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D809" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E809" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F809" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G809" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H809" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B810" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C810" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D810" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E810" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F810" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G810" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H810" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B811" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C811" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D811" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E811" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F811" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G811" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H811" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B812" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C812" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D812" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E812" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F812" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G812" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H812" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B813" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C813" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D813" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E813" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F813" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G813" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H813" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B814" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C814" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D814" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E814" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F814" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G814" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H814" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B815" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C815" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D815" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E815" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F815" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G815" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H815" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B816" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C816" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D816" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E816" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F816" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G816" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H816" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B817" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C817" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D817" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E817" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F817" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G817" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H817" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B818" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C818" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D818" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E818" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F818" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G818" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H818" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B819" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C819" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D819" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E819" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F819" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G819" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H819" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B820" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C820" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D820" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E820" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F820" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G820" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H820" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B821" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C821" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D821" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E821" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F821" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G821" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H821" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B822" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C822" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D822" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E822" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F822" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G822" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H822" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B823" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C823" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D823" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E823" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F823" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G823" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H823" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B824" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C824" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D824" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E824" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F824" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G824" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H824" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B825" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C825" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D825" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E825" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F825" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G825" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H825" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B826" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C826" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D826" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E826" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F826" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G826" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H826" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B827" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C827" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D827" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E827" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F827" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G827" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H827" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B828" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C828" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D828" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E828" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F828" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G828" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H828" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B829" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C829" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D829" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E829" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F829" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G829" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H829" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B830" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C830" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D830" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E830" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F830" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G830" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H830" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B831" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C831" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D831" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E831" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F831" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G831" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H831" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B832" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C832" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D832" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E832" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F832" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G832" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H832" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B833" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C833" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D833" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E833" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F833" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G833" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H833" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B834" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C834" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D834" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E834" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F834" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G834" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H834" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B835" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C835" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D835" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E835" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F835" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G835" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H835" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B836" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C836" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D836" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E836" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F836" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G836" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H836" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B837" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C837" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D837" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E837" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F837" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G837" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H837" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B838" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C838" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D838" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E838" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F838" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G838" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H838" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B839" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C839" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D839" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E839" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F839" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G839" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H839" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B840" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C840" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D840" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E840" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F840" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G840" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H840" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B841" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C841" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D841" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E841" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F841" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G841" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H841" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B842" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C842" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D842" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E842" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F842" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G842" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H842" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B843" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C843" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D843" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E843" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F843" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G843" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H843" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B844" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C844" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D844" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E844" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F844" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G844" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H844" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B845" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C845" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D845" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E845" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F845" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G845" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H845" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B846" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C846" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D846" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E846" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F846" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G846" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H846" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B847" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C847" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D847" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E847" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F847" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G847" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H847" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B848" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C848" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D848" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E848" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F848" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G848" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H848" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B849" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C849" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D849" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E849" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F849" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G849" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H849" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B850" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C850" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D850" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E850" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F850" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G850" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H850" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B851" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C851" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D851" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E851" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F851" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G851" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H851" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B852" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C852" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D852" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E852" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F852" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G852" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H852" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B853" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C853" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D853" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E853" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F853" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G853" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H853" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B854" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C854" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D854" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E854" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F854" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G854" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H854" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B855" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C855" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D855" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E855" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F855" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G855" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H855" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B856" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C856" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D856" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E856" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F856" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G856" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H856" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B857" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C857" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D857" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E857" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F857" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G857" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H857" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B858" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C858" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D858" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E858" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F858" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G858" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H858" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B859" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C859" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D859" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E859" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F859" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G859" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H859" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B860" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C860" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D860" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E860" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F860" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G860" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H860" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B861" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C861" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D861" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E861" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F861" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G861" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H861" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B862" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C862" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D862" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E862" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F862" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G862" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H862" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B863" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C863" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D863" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E863" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F863" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G863" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H863" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B864" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C864" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D864" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E864" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F864" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G864" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H864" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B865" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C865" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D865" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E865" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F865" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G865" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H865" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B866" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C866" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D866" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E866" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F866" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G866" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H866" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B867" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C867" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D867" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E867" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F867" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G867" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H867" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B868" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C868" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D868" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E868" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F868" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G868" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H868" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B869" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C869" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D869" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E869" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F869" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G869" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H869" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B870" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C870" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D870" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E870" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F870" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G870" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H870" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B871" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C871" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D871" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E871" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F871" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G871" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H871" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B872" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C872" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D872" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E872" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F872" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G872" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H872" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B873" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C873" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D873" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E873" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F873" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G873" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H873" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B874" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C874" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D874" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E874" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F874" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G874" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H874" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B875" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C875" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D875" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E875" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F875" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G875" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H875" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B876" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C876" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D876" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E876" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F876" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G876" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H876" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B877" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C877" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D877" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E877" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F877" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G877" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H877" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B878" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C878" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D878" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E878" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F878" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G878" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H878" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B879" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C879" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D879" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E879" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F879" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G879" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H879" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B880" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C880" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D880" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E880" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F880" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G880" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H880" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B881" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C881" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D881" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E881" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F881" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G881" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H881" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B882" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C882" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D882" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E882" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F882" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G882" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H882" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B883" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C883" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D883" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E883" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F883" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G883" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H883" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B884" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C884" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D884" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E884" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F884" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G884" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H884" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B885" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C885" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D885" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E885" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F885" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G885" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H885" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B886" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C886" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D886" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E886" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F886" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G886" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H886" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B887" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C887" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D887" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E887" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F887" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G887" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H887" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B888" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C888" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D888" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E888" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F888" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G888" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H888" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B889" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C889" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D889" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E889" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F889" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G889" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H889" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B890" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C890" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D890" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E890" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F890" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G890" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H890" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B891" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C891" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D891" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E891" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F891" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G891" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H891" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B892" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C892" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D892" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E892" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F892" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G892" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H892" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B893" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C893" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D893" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E893" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F893" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G893" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H893" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B894" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C894" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D894" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E894" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F894" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G894" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H894" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B895" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C895" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D895" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E895" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F895" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G895" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H895" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B896" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C896" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D896" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E896" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F896" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G896" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H896" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B897" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C897" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D897" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E897" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F897" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G897" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H897" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B898" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C898" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D898" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E898" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F898" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G898" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H898" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B899" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C899" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D899" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E899" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F899" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G899" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H899" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B900" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C900" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D900" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E900" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F900" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G900" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H900" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B901" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C901" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D901" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E901" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F901" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G901" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H901" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B902" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C902" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D902" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E902" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F902" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G902" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H902" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B903" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C903" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D903" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E903" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F903" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G903" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H903" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B904" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C904" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D904" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E904" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F904" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G904" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H904" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B905" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C905" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D905" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E905" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F905" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G905" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H905" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B906" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C906" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D906" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E906" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F906" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G906" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H906" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B907" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C907" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D907" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E907" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F907" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G907" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H907" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B908" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C908" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D908" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E908" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F908" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G908" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H908" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B909" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C909" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D909" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E909" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F909" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G909" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H909" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B910" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C910" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D910" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E910" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F910" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G910" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H910" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B911" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C911" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D911" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E911" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F911" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G911" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H911" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B912" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C912" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D912" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E912" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F912" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G912" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H912" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B913" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C913" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D913" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E913" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F913" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G913" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H913" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B914" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C914" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D914" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E914" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F914" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G914" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H914" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B915" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C915" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D915" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E915" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F915" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G915" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H915" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B916" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C916" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D916" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E916" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F916" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G916" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H916" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B917" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C917" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D917" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E917" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F917" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G917" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H917" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B918" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C918" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D918" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E918" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F918" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G918" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H918" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B919" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C919" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D919" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E919" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F919" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G919" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H919" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B920" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C920" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D920" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E920" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F920" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G920" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H920" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B921" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C921" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D921" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E921" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F921" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G921" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H921" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B922" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C922" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D922" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E922" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F922" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G922" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H922" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B923" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C923" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D923" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E923" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F923" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G923" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H923" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B924" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C924" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D924" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E924" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F924" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G924" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H924" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B925" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C925" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D925" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E925" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F925" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G925" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H925" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B926" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C926" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D926" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E926" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F926" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G926" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H926" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B927" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C927" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D927" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E927" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F927" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G927" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H927" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B928" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C928" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D928" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E928" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F928" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G928" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H928" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B929" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C929" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D929" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E929" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F929" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G929" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H929" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B930" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C930" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D930" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E930" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F930" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G930" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H930" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B931" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C931" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D931" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E931" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F931" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G931" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H931" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B932" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C932" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D932" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E932" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F932" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G932" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H932" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B933" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C933" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D933" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E933" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F933" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G933" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H933" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B934" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C934" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D934" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E934" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F934" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G934" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H934" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B935" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C935" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D935" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E935" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F935" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G935" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H935" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B936" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C936" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D936" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E936" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F936" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G936" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H936" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B937" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C937" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D937" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E937" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F937" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G937" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H937" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B938" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C938" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D938" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E938" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F938" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G938" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H938" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B939" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C939" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D939" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E939" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F939" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G939" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H939" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B940" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C940" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D940" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E940" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F940" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G940" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H940" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B941" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C941" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D941" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E941" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F941" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G941" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H941" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B942" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C942" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D942" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E942" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F942" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G942" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H942" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B943" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C943" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D943" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E943" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F943" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G943" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H943" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B944" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C944" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D944" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E944" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F944" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G944" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H944" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B945" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C945" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D945" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E945" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F945" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G945" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H945" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B946" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C946" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D946" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E946" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F946" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G946" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H946" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B947" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C947" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D947" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E947" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F947" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G947" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H947" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B948" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C948" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D948" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E948" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F948" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G948" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H948" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B949" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C949" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D949" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E949" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F949" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G949" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H949" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B950" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C950" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D950" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E950" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F950" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G950" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H950" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B951" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C951" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D951" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E951" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F951" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G951" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H951" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B952" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B953" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B954" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B955" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B956" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B957" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B958" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B959" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B960" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B961" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B962" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B963" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added filters for dragging documents
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66" count="17102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66" count="17534">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -1437,7 +1437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I963"/>
+  <dimension ref="A1:I987"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -26264,9 +26264,651 @@
     </row>
     <row r="963">
       <c r="A963" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B963" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C963" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D963" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E963" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F963" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G963" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H963" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B964" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C964" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D964" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E964" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F964" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G964" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H964" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B965" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C965" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D965" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E965" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F965" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G965" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H965" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B966" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C966" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D966" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E966" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F966" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G966" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H966" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B967" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C967" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D967" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E967" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F967" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G967" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H967" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B968" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C968" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D968" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E968" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F968" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G968" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H968" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B969" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C969" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D969" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E969" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F969" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G969" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H969" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B970" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C970" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D970" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E970" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F970" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G970" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H970" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B971" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C971" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D971" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E971" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F971" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G971" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H971" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B972" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C972" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D972" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E972" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F972" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G972" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H972" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B973" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C973" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D973" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E973" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F973" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G973" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H973" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B974" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C974" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D974" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E974" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F974" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G974" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H974" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B975" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C975" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D975" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E975" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F975" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G975" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H975" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B976" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C976" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D976" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E976" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F976" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G976" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H976" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B977" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C977" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D977" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E977" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F977" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G977" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H977" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B978" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C978" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D978" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E978" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F978" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G978" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H978" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B979" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C979" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D979" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E979" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F979" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G979" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H979" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B980" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C980" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D980" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E980" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F980" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G980" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H980" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B981" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C981" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D981" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E981" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F981" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G981" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H981" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B982" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C982" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D982" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E982" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F982" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G982" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H982" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B983" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C983" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D983" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E983" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F983" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G983" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H983" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B984" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C984" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D984" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E984" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F984" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G984" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H984" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B985" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C985" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D985" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E985" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F985" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G985" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H985" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B986" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C986" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D986" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E986" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F986" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G986" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H986" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B987" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C987" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D987" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E987" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F987" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G987" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H987" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the ability to read all rows from document and convert group of rows to columns
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16" count="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="12">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -55,10 +55,28 @@
     <t>Уганда, гасити вагнерів</t>
   </si>
   <si>
-    <t>01.01.2025Краківець</t>
+    <t>01.01.2025 Краківець</t>
   </si>
   <si>
     <t>01.01.2026 Подобовець</t>
+  </si>
+  <si>
+    <t>Тимків Віталій Дмитрович 1</t>
+  </si>
+  <si>
+    <t>А0000 1</t>
+  </si>
+  <si>
+    <t>Тимків Дмитро Віталійович 1</t>
+  </si>
+  <si>
+    <t>Уганда, гасити вагнерів 1</t>
+  </si>
+  <si>
+    <t>01.01.2025 Краківець 1</t>
+  </si>
+  <si>
+    <t>01.01.2026 Подобовець 1</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1305,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1348,9 +1366,9 @@
       <c r="I2" s="7"/>
     </row>
     <row r="3" ht="18" customHeight="1">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="9">
         <f>ROW(A1)</f>
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="9">
         <v>2</v>
@@ -1381,22 +1399,22 @@
       <c r="A4" s="9" t="n">
         <v>1.0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1404,460 +1422,23 @@
       <c r="A5" s="9" t="n">
         <v>2.0</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="9" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="9" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="9" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="9" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="9" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="9" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="9" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="9" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="9" t="n">
-        <v>15.0</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="n">
-        <v>16.0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="9" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="9" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="9" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>15</v>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added reading config from yaml file.
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="36">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -41,6 +41,42 @@
   </si>
   <si>
     <t>Фактично</t>
+  </si>
+  <si>
+    <t>Тимків Віталій Дмитрович</t>
+  </si>
+  <si>
+    <t>А0000</t>
+  </si>
+  <si>
+    <t>Тимків Дмитро Віталійович</t>
+  </si>
+  <si>
+    <t>Уганда, гасити вагнерів</t>
+  </si>
+  <si>
+    <t>01.01.2025 Краківець</t>
+  </si>
+  <si>
+    <t>01.01.2026 Подобовець</t>
+  </si>
+  <si>
+    <t>Тимків Віталій Дмитрович 1</t>
+  </si>
+  <si>
+    <t>А0000 1</t>
+  </si>
+  <si>
+    <t>Тимків Дмитро Віталійович 1</t>
+  </si>
+  <si>
+    <t>Уганда, гасити вагнерів 1</t>
+  </si>
+  <si>
+    <t>01.01.2025 Краківець 1</t>
+  </si>
+  <si>
+    <t>01.01.2026 Подобовець 1</t>
   </si>
 </sst>
 </file>
@@ -1269,22 +1305,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="8.85156"/>
+    <col min="2" max="2" customWidth="true" style="1" width="35.5"/>
+    <col min="3" max="3" customWidth="true" style="1" width="30.1719"/>
+    <col min="4" max="4" customWidth="true" style="1" width="38.8516"/>
+    <col min="5" max="5" customWidth="true" style="1" width="34.3516"/>
+    <col min="6" max="6" customWidth="true" style="1" width="17.1719"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.0"/>
+    <col min="8" max="8" customWidth="true" style="1" width="13.5"/>
+    <col min="9" max="9" customWidth="true" style="1" width="17.5"/>
+    <col min="10" max="16384" customWidth="true" style="1" width="8.85156"/>
   </cols>
   <sheetData>
     <row r="1" ht="64.2" customHeight="1">
@@ -1357,6 +1393,144 @@
       </c>
       <c r="I3" s="9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logger to log4j2.xml
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -41,42 +41,6 @@
   </si>
   <si>
     <t>Фактично</t>
-  </si>
-  <si>
-    <t>Тимків Віталій Дмитрович</t>
-  </si>
-  <si>
-    <t>А0000</t>
-  </si>
-  <si>
-    <t>Тимків Дмитро Віталійович</t>
-  </si>
-  <si>
-    <t>Уганда, гасити вагнерів</t>
-  </si>
-  <si>
-    <t>01.01.2025 Краківець</t>
-  </si>
-  <si>
-    <t>01.01.2026 Подобовець</t>
-  </si>
-  <si>
-    <t>Тимків Віталій Дмитрович 1</t>
-  </si>
-  <si>
-    <t>А0000 1</t>
-  </si>
-  <si>
-    <t>Тимків Дмитро Віталійович 1</t>
-  </si>
-  <si>
-    <t>Уганда, гасити вагнерів 1</t>
-  </si>
-  <si>
-    <t>01.01.2025 Краківець 1</t>
-  </si>
-  <si>
-    <t>01.01.2026 Подобовець 1</t>
   </si>
 </sst>
 </file>
@@ -1305,22 +1269,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="8.85156"/>
-    <col min="2" max="2" customWidth="true" style="1" width="35.5"/>
-    <col min="3" max="3" customWidth="true" style="1" width="30.1719"/>
-    <col min="4" max="4" customWidth="true" style="1" width="38.8516"/>
-    <col min="5" max="5" customWidth="true" style="1" width="34.3516"/>
-    <col min="6" max="6" customWidth="true" style="1" width="17.1719"/>
-    <col min="7" max="7" customWidth="true" style="1" width="14.0"/>
-    <col min="8" max="8" customWidth="true" style="1" width="13.5"/>
-    <col min="9" max="9" customWidth="true" style="1" width="17.5"/>
-    <col min="10" max="16384" customWidth="true" style="1" width="8.85156"/>
+    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.1719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.3516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1719" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="64.2" customHeight="1">
@@ -1393,144 +1357,6 @@
       </c>
       <c r="I3" s="9">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="9" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="9" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read config file either from jar or from file system
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="96">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -41,6 +41,42 @@
   </si>
   <si>
     <t>Фактично</t>
+  </si>
+  <si>
+    <t>Тимків Віталій Дмитрович</t>
+  </si>
+  <si>
+    <t>А0000</t>
+  </si>
+  <si>
+    <t>Тимків Дмитро Віталійович</t>
+  </si>
+  <si>
+    <t>Уганда, гасити вагнерів</t>
+  </si>
+  <si>
+    <t>01.01.2025 Краківець</t>
+  </si>
+  <si>
+    <t>01.01.2026 Подобовець</t>
+  </si>
+  <si>
+    <t>Тимків Віталій Дмитрович 1</t>
+  </si>
+  <si>
+    <t>А0000 1</t>
+  </si>
+  <si>
+    <t>Тимків Дмитро Віталійович 1</t>
+  </si>
+  <si>
+    <t>Уганда, гасити вагнерів 1</t>
+  </si>
+  <si>
+    <t>01.01.2025 Краківець 1</t>
+  </si>
+  <si>
+    <t>01.01.2026 Подобовець 1</t>
   </si>
 </sst>
 </file>
@@ -1269,22 +1305,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1719" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="8.85156"/>
+    <col min="2" max="2" customWidth="true" style="1" width="35.5"/>
+    <col min="3" max="3" customWidth="true" style="1" width="30.1719"/>
+    <col min="4" max="4" customWidth="true" style="1" width="38.8516"/>
+    <col min="5" max="5" customWidth="true" style="1" width="34.3516"/>
+    <col min="6" max="6" customWidth="true" style="1" width="17.1719"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.0"/>
+    <col min="8" max="8" customWidth="true" style="1" width="13.5"/>
+    <col min="9" max="9" customWidth="true" style="1" width="17.5"/>
+    <col min="10" max="16384" customWidth="true" style="1" width="8.85156"/>
   </cols>
   <sheetData>
     <row r="1" ht="64.2" customHeight="1">
@@ -1357,6 +1393,374 @@
       </c>
       <c r="I3" s="9">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored code to read both types of documents: doc and docx.
</commit_message>
<xml_diff>
--- a/w2e-core/src/test/resources/output_data/journal.xlsx
+++ b/w2e-core/src/test/resources/output_data/journal.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22" count="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23" count="168">
   <si>
     <t>№ з/п, дата</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>01.01.2026 Подобовець 1</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1305,7 +1308,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1763,6 +1766,190 @@
         <v>21</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="9" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B24" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B25" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="F25" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B26" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s" s="9">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s" s="9">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B27" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="D27" t="s" s="9">
+        <v>18</v>
+      </c>
+      <c r="E27" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="F27" t="s" s="9">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s" s="9">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="I1:I2"/>

</xml_diff>